<commit_message>
updated code for Random forest classifier
</commit_message>
<xml_diff>
--- a/data_/accuracies.xlsx
+++ b/data_/accuracies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Upswing Pursuit\Courses\Udacity\ML Engineer Nanodegree\Project\predict-suicides-to-save-lives\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Upswing Pursuit\Courses\Udacity\ML Engineer Nanodegree\Project\predict-suicides-to-save-lives\data_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C6FC17-E78C-4D9B-8076-8D638952A5CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3228C7CC-37AE-4AAE-8B50-1E4C2FD97AD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0.67281105990783407</v>
+        <v>0.68018433179723503</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -511,7 +511,7 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>0.67281105990783407</v>
+        <v>0.69216589861751154</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -522,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>0.68663594470046085</v>
+        <v>0.69216589861751154</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -533,7 +533,7 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>0.67900092506938026</v>
+        <v>0.68663594470046085</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>

</xml_diff>